<commit_message>
as / Updating Sprint plan
</commit_message>
<xml_diff>
--- a/docs/Agile_Sprint_Plan.xlsx
+++ b/docs/Agile_Sprint_Plan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aarthy_Kidambi_Sekar\Documents\School\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aarthy_Kidambi_Sekar\Documents\School\SlidingPuzzle\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="42">
   <si>
     <t>Sprint</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>Final Documentation preparation</t>
+  </si>
+  <si>
+    <t>Logout</t>
   </si>
 </sst>
 </file>
@@ -582,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1074,25 +1077,40 @@
       <c r="F25" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G25" s="8" t="s">
+      <c r="G25" s="15" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="12" t="s">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="3"/>
+      <c r="G26" s="12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="E26" s="7" t="str">
+      <c r="E27" s="7" t="str">
         <f>'Team members'!A1</f>
         <v>Kidambi Sekar, Aarthy (a_k196)</v>
       </c>
-      <c r="F26" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G26" s="15" t="s">
+      <c r="F27" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G27" s="15" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>